<commit_message>
Se modifico el archivo del lab01
</commit_message>
<xml_diff>
--- a/lab01/Libro1.xlsx
+++ b/lab01/Libro1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\reposInventario2025\lab01\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\recuperado\reposIventario2025\lab01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5D9DD33A-3318-4545-8CA6-1141A11C69A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9155DE4C-DBAB-48E2-82F8-CC32B32123DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{32B61811-5C45-4032-8DEA-C0285D7E24E8}"/>
   </bookViews>
@@ -56,7 +56,7 @@
     <t>descripcion</t>
   </si>
   <si>
-    <t>PC DELL ALL IN ONE CORE I7</t>
+    <t>PC DELL ALL IN ONE CORE I9 mem 32gb</t>
   </si>
 </sst>
 </file>
@@ -431,7 +431,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C3" sqref="C3:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>